<commit_message>
add more example files
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/ExcelFunctions2007-7thonline.xlsx
+++ b/src/main/webapp/book/ExcelFunctions2007-7thonline.xlsx
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>name-range formula</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>OR</t>
-  </si>
-  <si>
-    <t>over 10</t>
   </si>
   <si>
     <t>Text</t>
@@ -389,43 +386,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <condense val="0"/>
@@ -853,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="D149" sqref="D149"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -869,98 +830,82 @@
     <col min="9" max="9" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="5" t="b">
         <f>ISBLANK(B5)</f>
         <v>0</v>
       </c>
-      <c r="C4" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" t="str">
-        <f>IF(B4=C4,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="5"/>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="b">
         <f>ISERROR(B12)</f>
         <v>1</v>
       </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="str">
-        <f>IF(B11=C11,"T","WARN")</f>
-        <v>T</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="5" t="e">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -971,18 +916,11 @@
     </row>
     <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" t="b">
         <f>ISNA(B20)</f>
         <v>0</v>
-      </c>
-      <c r="C19" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" t="str">
-        <f>IF(B19=C19,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1006,18 +944,11 @@
     </row>
     <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" t="b">
         <f>ISNUMBER(B26)</f>
         <v>1</v>
-      </c>
-      <c r="C25" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" t="str">
-        <f>IF(B25=C25,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1041,24 +972,17 @@
     </row>
     <row r="31" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" t="b">
         <f>ISTEXT(B32)</f>
         <v>1</v>
       </c>
-      <c r="C31" t="b">
-        <v>1</v>
-      </c>
-      <c r="D31" t="str">
-        <f>IF(B31=C31,"T","WARN")</f>
-        <v>T</v>
-      </c>
     </row>
     <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1074,9 +998,7 @@
       <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C35" s="1"/>
       <c r="D35" s="10"/>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1086,13 +1008,6 @@
       <c r="B37" s="5" t="b">
         <f>AND(TRUE, TRUE)</f>
         <v>1</v>
-      </c>
-      <c r="C37" t="b">
-        <v>1</v>
-      </c>
-      <c r="D37" t="str">
-        <f>IF(B37=C37,"T","WARN")</f>
-        <v>T</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1115,13 +1030,6 @@
         <f>IF(B42&gt;10,"over 10", "less than 10")</f>
         <v>over 10</v>
       </c>
-      <c r="C41" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" t="str">
-        <f>IF(B41=C41,"T","WARN")</f>
-        <v>T</v>
-      </c>
     </row>
     <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
@@ -1140,13 +1048,6 @@
         <f>IFERROR(B45/C45,"error")</f>
         <v>6</v>
       </c>
-      <c r="C44">
-        <v>6</v>
-      </c>
-      <c r="D44" t="str">
-        <f>IF(B44=C44,"T","WARN")</f>
-        <v>T</v>
-      </c>
     </row>
     <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
@@ -1175,13 +1076,6 @@
         <f>OR(1+1=1,2+2=5)</f>
         <v>0</v>
       </c>
-      <c r="C49" t="b">
-        <v>0</v>
-      </c>
-      <c r="D49" t="str">
-        <f>IF(B49=C49,"T","WARN")</f>
-        <v>T</v>
-      </c>
     </row>
     <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
@@ -1194,7 +1088,7 @@
     </row>
     <row r="53" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>9</v>
@@ -1218,14 +1112,14 @@
     </row>
     <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B58" s="14" t="str">
         <f>LOOKUP(4.19,B59:B63,C59:C63)</f>
         <v>orange</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D58" t="str">
         <f>IF(B58=C58,"T","WARN")</f>
@@ -1238,7 +1132,7 @@
         <v>4.1399999999999997</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1247,7 +1141,7 @@
         <v>4.1900000000000004</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1256,7 +1150,7 @@
         <v>5.17</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1265,7 +1159,7 @@
         <v>5.77</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1274,7 +1168,7 @@
         <v>6.39</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1631,7 +1525,7 @@
     </row>
     <row r="104" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B104" s="16" t="s">
         <v>9</v>
@@ -1650,7 +1544,7 @@
     </row>
     <row r="108" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1690,7 +1584,7 @@
     </row>
     <row r="112" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B112">
         <f>COUNT(B113:H113)</f>
@@ -1707,7 +1601,7 @@
     <row r="113" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
       <c r="B113" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C113" s="13">
         <v>39672</v>
@@ -1730,7 +1624,7 @@
     </row>
     <row r="115" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B115">
         <f>MAX(B116:F116)</f>
@@ -1774,7 +1668,7 @@
     </row>
     <row r="121" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A121" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>9</v>
@@ -1794,14 +1688,14 @@
     </row>
     <row r="125" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A125" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B125" t="str">
         <f>CONCATENATE(B126,C126)</f>
         <v>ZK</v>
       </c>
       <c r="C125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D125" t="str">
         <f>IF(B125=C125,"T","WARN")</f>
@@ -1811,10 +1705,10 @@
     <row r="126" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A126" s="20"/>
       <c r="B126" t="s">
+        <v>24</v>
+      </c>
+      <c r="C126" t="s">
         <v>25</v>
-      </c>
-      <c r="C126" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="127" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -1822,14 +1716,14 @@
     </row>
     <row r="128" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A128" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B128" t="str">
         <f>LEFT(B129,4)</f>
         <v xml:space="preserve">東 京 </v>
       </c>
       <c r="C128" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D128" t="str">
         <f>IF(B128=C128,"T","WARN")</f>
@@ -1839,19 +1733,19 @@
     <row r="129" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A129" s="20"/>
       <c r="B129" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A130" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B130" t="str">
         <f>LEFTB(B129,4)</f>
         <v xml:space="preserve">東 京 </v>
       </c>
       <c r="C130" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D130" t="str">
         <f>IF(B130=C130,"T","WARN")</f>
@@ -1866,14 +1760,14 @@
     </row>
     <row r="133" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A133" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B133" t="str">
         <f>RIGHT(B134,5)</f>
         <v>Price</v>
       </c>
       <c r="C133" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D133" t="str">
         <f>IF(B133=C133,"T","WARN")</f>
@@ -1883,19 +1777,19 @@
     <row r="134" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="20"/>
       <c r="B134" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B135" t="str">
         <f>RIGHTB(B134,5)</f>
         <v>Price</v>
       </c>
       <c r="C135" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D135" t="str">
         <f>IF(B135=C135,"T","WARN")</f>
@@ -1907,7 +1801,7 @@
     </row>
     <row r="137" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A137" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B137">
         <f>SEARCH("Price",B138)</f>
@@ -1924,7 +1818,7 @@
     <row r="138" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A138" s="20"/>
       <c r="B138" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -1932,14 +1826,14 @@
     </row>
     <row r="140" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A140" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B140" t="str">
         <f>"Date: " &amp; TEXT(B141,"yyyy-mm-dd")</f>
         <v>Date: 2007-08-06</v>
       </c>
       <c r="C140" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D140" t="str">
         <f>IF(B140=C140,"T","WARN")</f>
@@ -1957,14 +1851,14 @@
     </row>
     <row r="143" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B143" t="str">
         <f>TRIM(" revenue in quarter 1 ")</f>
         <v>revenue in quarter 1</v>
       </c>
       <c r="C143" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D143" t="str">
         <f>IF(B143=C143,"T","WARN")</f>
@@ -1987,7 +1881,7 @@
     </row>
     <row r="148" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B148" s="14">
         <f>VALUE("1,000")</f>
@@ -2239,52 +2133,52 @@
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <conditionalFormatting sqref="D2 D11 D14 D17 D19 D22 D25 D27 D4:D8">
-    <cfRule type="cellIs" dxfId="12" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29 D31 D34">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37 D39 D41 D44 D47 D49">
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55 D58:D63">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69 D72 D74:D75 D79 D81 D87 D97">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D106 D109">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D112">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D115">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D123:D149">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"WARN"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>